<commit_message>
New reports and charts
</commit_message>
<xml_diff>
--- a/reports/Angola_export_top_5_partners_cols.xlsx
+++ b/reports/Angola_export_top_5_partners_cols.xlsx
@@ -692,37 +692,37 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>0.02557541560953335</v>
+        <v>0.02557541560474827</v>
       </c>
       <c r="D6">
-        <v>0.4445853536651129</v>
+        <v>0.4445853535819324</v>
       </c>
       <c r="E6">
-        <v>0.01589511551552907</v>
+        <v>0.01589511551255514</v>
       </c>
       <c r="F6">
-        <v>0.1062446241465069</v>
+        <v>0.1062446241266289</v>
       </c>
       <c r="G6">
-        <v>0.06629932979857632</v>
+        <v>0.06629932978617192</v>
       </c>
       <c r="H6">
-        <v>0.03034309353729176</v>
+        <v>0.03034309353161467</v>
       </c>
       <c r="I6">
-        <v>0.03712770700742384</v>
+        <v>0.03712770700047736</v>
       </c>
       <c r="J6">
-        <v>0.01887325925243592</v>
+        <v>0.01887325924890479</v>
       </c>
       <c r="K6">
-        <v>0.004397619981854402</v>
+        <v>0.004397619981031621</v>
       </c>
       <c r="L6">
-        <v>0.132868196435513</v>
+        <v>0.1328681964106538</v>
       </c>
       <c r="M6">
-        <v>0.01635929666379739</v>
+        <v>0.01635929666073662</v>
       </c>
       <c r="N6">
         <v>1930696671</v>
@@ -914,37 +914,37 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>0.01412633961513851</v>
+        <v>0.01412633959113824</v>
       </c>
       <c r="D9">
-        <v>0.4344733953284274</v>
+        <v>0.4344733945902689</v>
       </c>
       <c r="E9">
-        <v>0.04372751189025071</v>
+        <v>0.04372751181595886</v>
       </c>
       <c r="F9">
-        <v>0.08606047378102122</v>
+        <v>0.0860604736348068</v>
       </c>
       <c r="G9">
-        <v>0.03702518791081145</v>
+        <v>0.03702518784790666</v>
       </c>
       <c r="H9">
-        <v>0.03438882485105956</v>
+        <v>0.03438882479263388</v>
       </c>
       <c r="I9">
-        <v>0.0364979155645691</v>
+        <v>0.03649791550256013</v>
       </c>
       <c r="J9">
-        <v>0.06084851519600279</v>
+        <v>0.06084851509262281</v>
       </c>
       <c r="K9">
-        <v>0.004228369035225846</v>
+        <v>0.004228369028041961</v>
       </c>
       <c r="L9">
-        <v>0.07920342855298187</v>
+        <v>0.0792034284184174</v>
       </c>
       <c r="M9">
-        <v>0.02868902530010028</v>
+        <v>0.02868902525135841</v>
       </c>
       <c r="N9">
         <v>520271665</v>
@@ -1284,37 +1284,37 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>1.606722893964805E-06</v>
+        <v>1.606721330475717E-06</v>
       </c>
       <c r="D14">
-        <v>0.6146636139554205</v>
+        <v>0.6146630158312157</v>
       </c>
       <c r="E14">
-        <v>0.02074250956079669</v>
+        <v>0.02074248937642795</v>
       </c>
       <c r="F14">
-        <v>0.08423488957802745</v>
+        <v>0.08423480760973587</v>
       </c>
       <c r="G14">
-        <v>0.02076997192236546</v>
+        <v>0.02076995171127332</v>
       </c>
       <c r="H14">
-        <v>0.0185242580834723</v>
+        <v>0.01852424005766618</v>
       </c>
       <c r="I14">
-        <v>0.002505255585279392</v>
+        <v>0.002505253147435391</v>
       </c>
       <c r="J14">
-        <v>0.02609725446512716</v>
+        <v>0.02609722907009935</v>
       </c>
       <c r="K14">
-        <v>0.05240476294158734</v>
+        <v>0.05240471194693522</v>
       </c>
       <c r="L14">
-        <v>0.0207145958123928</v>
+        <v>0.0207145756551867</v>
       </c>
       <c r="M14">
-        <v>0.04241063180190716</v>
+        <v>0.04241059053246345</v>
       </c>
       <c r="N14">
         <v>38576.52</v>

</xml_diff>